<commit_message>
QRCode image size dynamic, table UI update
</commit_message>
<xml_diff>
--- a/app/src/assets/QR Code template.xlsx
+++ b/app/src/assets/QR Code template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rachiitt/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\qrCode\app\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72306A6-24CB-1147-9CBE-8231394BBBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47347FCB-5E7B-4100-B091-59238A468F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28020" windowHeight="15220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>First name</t>
   </si>
@@ -44,12 +43,6 @@
     <t>Fax number</t>
   </si>
   <si>
-    <t>Phone number</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Contact number</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -77,41 +70,17 @@
     <t>Website</t>
   </si>
   <si>
-    <t>Pawan Kumar</t>
-  </si>
-  <si>
-    <t>Gautam</t>
-  </si>
-  <si>
-    <t>pawan.kumar@augtrans.com</t>
-  </si>
-  <si>
-    <t>Augmented transformations pvt ltd</t>
-  </si>
-  <si>
-    <t>full stack developer</t>
-  </si>
-  <si>
-    <t>barra</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> kanpur</t>
-  </si>
-  <si>
-    <t>up</t>
-  </si>
-  <si>
-    <t>india</t>
-  </si>
-  <si>
-    <t>google.co.uk</t>
+    <t>Contact number</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Phone number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -133,6 +102,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -148,7 +133,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -156,16 +141,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -506,15 +504,15 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.95"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.375" customWidth="1"/>
     <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.5" bestFit="1" customWidth="1"/>
@@ -527,101 +525,75 @@
     <col min="14" max="14" width="13.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.95">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" ht="18.95">
-      <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
+    <row r="2" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="1">
-        <v>9625028099</v>
-      </c>
-      <c r="E2" s="1">
-        <v>9625028099</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="1">
-        <v>208001</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="18.95">
+    <row r="3" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -632,7 +604,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" ht="18.95">
+    <row r="4" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -649,7 +621,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" ht="18.95">
+    <row r="5" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -666,7 +638,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="18.95">
+    <row r="6" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -683,7 +655,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" ht="18.95">
+    <row r="7" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -700,7 +672,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" ht="18.95">
+    <row r="8" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>

</xml_diff>